<commit_message>
Added login details excel sheet
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NomveloZuluProvidenc\Documents\Projects\SauceDemoAssessment1\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C185E61F-28C0-404C-8543-73C9667C5E23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9459FB00-CF93-43E0-A11F-7B765E0F4F3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10380" xr2:uid="{F8890393-857F-4E3E-8459-69860701986F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10380" activeTab="1" xr2:uid="{F8890393-857F-4E3E-8459-69860701986F}"/>
   </bookViews>
   <sheets>
     <sheet name="User Details" sheetId="1" r:id="rId1"/>
+    <sheet name="Login Details" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Mvelo</t>
   </si>
@@ -61,13 +62,34 @@
   </si>
   <si>
     <t>PostalCode</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +101,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,10 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2216C7A-250E-42BE-BC9B-0EFD6B4B4EA8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -520,4 +549,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A220E87B-3E8A-4F6B-BD61-05B41F66AD57}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>